<commit_message>
tukar task load data dengan preprocessing data
</commit_message>
<xml_diff>
--- a/sprint_project.xlsx
+++ b/sprint_project.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24326"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24430"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\DATA KULIAH\SEMESTER 7\Pembelajaran Mesin\Praktikum\Tugas_Praktikum_ML_A_297-233\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DA75CD63-1C90-46B1-950F-FB0A457DFFD1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AAC1EFB7-D875-4F76-A9CE-4439E6032C7F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="576" yWindow="696" windowWidth="17280" windowHeight="8964" xr2:uid="{5C1D3006-E29B-4E8A-AA24-3CECFF9100A6}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{5C1D3006-E29B-4E8A-AA24-3CECFF9100A6}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -497,7 +497,7 @@
   <dimension ref="A1:F13"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C14" sqref="C14"/>
+      <selection activeCell="F2" sqref="F2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -541,7 +541,7 @@
         <v>25</v>
       </c>
       <c r="E2" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="F2" t="s">
         <v>32</v>
@@ -558,7 +558,7 @@
         <v>25</v>
       </c>
       <c r="E3" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="F3" t="s">
         <v>32</v>

</xml_diff>

<commit_message>
mengubah status task preprocessing data menjadi ongoing
</commit_message>
<xml_diff>
--- a/sprint_project.xlsx
+++ b/sprint_project.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\DATA KULIAH\SEMESTER 7\Pembelajaran Mesin\Praktikum\Tugas_Praktikum_ML_A_297-233\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AAC1EFB7-D875-4F76-A9CE-4439E6032C7F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{29EB0075-987D-41D3-B495-56FF24065B71}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{5C1D3006-E29B-4E8A-AA24-3CECFF9100A6}"/>
   </bookViews>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="71" uniqueCount="34">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="71" uniqueCount="35">
   <si>
     <t>TASK</t>
   </si>
@@ -128,6 +128,9 @@
   </si>
   <si>
     <t>14 Desember 2021</t>
+  </si>
+  <si>
+    <t>ONGOING</t>
   </si>
 </sst>
 </file>
@@ -497,7 +500,7 @@
   <dimension ref="A1:F13"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F2" sqref="F2"/>
+      <selection activeCell="G4" sqref="G4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -561,7 +564,7 @@
         <v>20</v>
       </c>
       <c r="F3" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.3">

</xml_diff>

<commit_message>
changing naufal's status on sprint_project
</commit_message>
<xml_diff>
--- a/sprint_project.xlsx
+++ b/sprint_project.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\DATA KULIAH\SEMESTER 7\Pembelajaran Mesin\Praktikum\Tugas_Praktikum_ML_A_297-233\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\DATA 1\ARSIP TUGAS\ARSIP UMM\TUGAS KULIAH TEKNIK INFORMATIKA UMM\SEMESTER 7\PEMBELAJARAN MESIN 7A\MODUL PRAKTIKUM\TUGAS PRAK ML KELOMPOK\Tugas_Praktikum_ML_A_297-233\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AAC1EFB7-D875-4F76-A9CE-4439E6032C7F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2F428C9A-A858-45B0-9F16-EE44CF2B7F08}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{5C1D3006-E29B-4E8A-AA24-3CECFF9100A6}"/>
+    <workbookView xWindow="2160" yWindow="2160" windowWidth="17280" windowHeight="8964" xr2:uid="{5C1D3006-E29B-4E8A-AA24-3CECFF9100A6}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="71" uniqueCount="34">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="71" uniqueCount="35">
   <si>
     <t>TASK</t>
   </si>
@@ -128,6 +128,9 @@
   </si>
   <si>
     <t>14 Desember 2021</t>
+  </si>
+  <si>
+    <t>DONE</t>
   </si>
 </sst>
 </file>
@@ -497,7 +500,7 @@
   <dimension ref="A1:F13"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F2" sqref="F2"/>
+      <selection activeCell="F3" sqref="F3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -544,7 +547,7 @@
         <v>21</v>
       </c>
       <c r="F2" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.3">

</xml_diff>

<commit_message>
ubah status task preprocessing data
</commit_message>
<xml_diff>
--- a/sprint_project.xlsx
+++ b/sprint_project.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\DATA 1\ARSIP TUGAS\ARSIP UMM\TUGAS KULIAH TEKNIK INFORMATIKA UMM\SEMESTER 7\PEMBELAJARAN MESIN 7A\MODUL PRAKTIKUM\TUGAS PRAK ML KELOMPOK\Tugas_Praktikum_ML_A_297-233\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\DATA KULIAH\SEMESTER 7\Pembelajaran Mesin\Praktikum\Tugas_Praktikum_ML_A_297-233\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2F428C9A-A858-45B0-9F16-EE44CF2B7F08}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E71A405D-3D1C-459A-94EB-BAE285E82239}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2160" yWindow="2160" windowWidth="17280" windowHeight="8964" xr2:uid="{5C1D3006-E29B-4E8A-AA24-3CECFF9100A6}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{5C1D3006-E29B-4E8A-AA24-3CECFF9100A6}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="71" uniqueCount="35">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="72" uniqueCount="36">
   <si>
     <t>TASK</t>
   </si>
@@ -131,6 +131,9 @@
   </si>
   <si>
     <t>DONE</t>
+  </si>
+  <si>
+    <t>25 Oktober 2021</t>
   </si>
 </sst>
 </file>
@@ -500,7 +503,7 @@
   <dimension ref="A1:F13"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F3" sqref="F3"/>
+      <selection activeCell="E18" sqref="E18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -560,11 +563,14 @@
       <c r="C3" t="s">
         <v>25</v>
       </c>
+      <c r="D3" t="s">
+        <v>35</v>
+      </c>
       <c r="E3" t="s">
         <v>20</v>
       </c>
       <c r="F3" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.3">

</xml_diff>

<commit_message>
report pada sprint_project (mengisi tanggal pada task 'load data'
</commit_message>
<xml_diff>
--- a/sprint_project.xlsx
+++ b/sprint_project.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\DATA KULIAH\SEMESTER 7\Pembelajaran Mesin\Praktikum\Tugas_Praktikum_ML_A_297-233\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E71A405D-3D1C-459A-94EB-BAE285E82239}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D7B04057-ADE1-4D69-8655-4936CC963990}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{5C1D3006-E29B-4E8A-AA24-3CECFF9100A6}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="1" xr2:uid="{5C1D3006-E29B-4E8A-AA24-3CECFF9100A6}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="72" uniqueCount="36">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="78" uniqueCount="41">
   <si>
     <t>TASK</t>
   </si>
@@ -134,6 +134,21 @@
   </si>
   <si>
     <t>25 Oktober 2021</t>
+  </si>
+  <si>
+    <t>16 Oktober 2021</t>
+  </si>
+  <si>
+    <t>Menambah tanggal pada tanggal selesai task "load data"</t>
+  </si>
+  <si>
+    <t>Selesai</t>
+  </si>
+  <si>
+    <t>tanggal selesai pada task "load data" belum ditulis</t>
+  </si>
+  <si>
+    <t>Muhammad Fadhlan</t>
   </si>
 </sst>
 </file>
@@ -181,11 +196,14 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="15" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -502,8 +520,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7C6EBB1A-5C24-4770-A58A-F4BAF81FE81F}">
   <dimension ref="A1:F13"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E18" sqref="E18"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D2" sqref="D2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -546,6 +564,9 @@
       <c r="C2" t="s">
         <v>25</v>
       </c>
+      <c r="D2" t="s">
+        <v>36</v>
+      </c>
       <c r="E2" t="s">
         <v>21</v>
       </c>
@@ -751,10 +772,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A1014770-38FB-4B19-AD2D-C94E0AFBC5C4}">
-  <dimension ref="A1:E1"/>
+  <dimension ref="A1:E2"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C8" sqref="C8"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C6" sqref="C6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -783,6 +804,23 @@
         <v>17</v>
       </c>
     </row>
+    <row r="2" spans="1:5" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="A2" t="s">
+        <v>26</v>
+      </c>
+      <c r="B2" s="4" t="s">
+        <v>39</v>
+      </c>
+      <c r="C2" t="s">
+        <v>38</v>
+      </c>
+      <c r="D2" s="4" t="s">
+        <v>37</v>
+      </c>
+      <c r="E2" t="s">
+        <v>40</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
task aug data done, model with aug done, model eval done, and add task image processing
</commit_message>
<xml_diff>
--- a/sprint_project.xlsx
+++ b/sprint_project.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24430"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24527"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\DATA KULIAH\SEMESTER 7\Pembelajaran Mesin\Praktikum\Tugas_Praktikum_ML_A_297-233\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Fadhlan\Pembelajaran Mesin\Tugas_Praktikum_ML_A_297-233\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D7B04057-ADE1-4D69-8655-4936CC963990}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BDA035D8-B585-426F-97E0-466EB705D078}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="1" xr2:uid="{5C1D3006-E29B-4E8A-AA24-3CECFF9100A6}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{5C1D3006-E29B-4E8A-AA24-3CECFF9100A6}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="78" uniqueCount="41">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="86" uniqueCount="44">
   <si>
     <t>TASK</t>
   </si>
@@ -149,6 +149,15 @@
   </si>
   <si>
     <t>Muhammad Fadhlan</t>
+  </si>
+  <si>
+    <t>8 Nopember 2021</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ADD IMAGE PROCESSING </t>
+  </si>
+  <si>
+    <t>ON GOING</t>
   </si>
 </sst>
 </file>
@@ -518,10 +527,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7C6EBB1A-5C24-4770-A58A-F4BAF81FE81F}">
-  <dimension ref="A1:F13"/>
+  <dimension ref="A1:F14"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D2" sqref="D2"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F9" sqref="F9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -604,11 +613,14 @@
       <c r="C4" t="s">
         <v>26</v>
       </c>
+      <c r="D4" t="s">
+        <v>26</v>
+      </c>
       <c r="E4" t="s">
         <v>20</v>
       </c>
       <c r="F4" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.3">
@@ -638,11 +650,14 @@
       <c r="C6" s="3" t="s">
         <v>27</v>
       </c>
+      <c r="D6" t="s">
+        <v>26</v>
+      </c>
       <c r="E6" t="s">
         <v>20</v>
       </c>
       <c r="F6" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.3">
@@ -655,16 +670,19 @@
       <c r="C7" t="s">
         <v>28</v>
       </c>
+      <c r="D7" t="s">
+        <v>41</v>
+      </c>
       <c r="E7" t="s">
         <v>21</v>
       </c>
       <c r="F7" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
-        <v>22</v>
+        <v>42</v>
       </c>
       <c r="B8" t="s">
         <v>28</v>
@@ -676,12 +694,12 @@
         <v>20</v>
       </c>
       <c r="F8" t="s">
-        <v>32</v>
+        <v>43</v>
       </c>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
-        <v>9</v>
+        <v>22</v>
       </c>
       <c r="B9" t="s">
         <v>28</v>
@@ -690,7 +708,7 @@
         <v>29</v>
       </c>
       <c r="E9" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="F9" t="s">
         <v>32</v>
@@ -698,13 +716,13 @@
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B10" t="s">
+        <v>28</v>
+      </c>
+      <c r="C10" t="s">
         <v>29</v>
-      </c>
-      <c r="C10" t="s">
-        <v>30</v>
       </c>
       <c r="E10" t="s">
         <v>21</v>
@@ -715,7 +733,7 @@
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B11" t="s">
         <v>29</v>
@@ -724,7 +742,7 @@
         <v>30</v>
       </c>
       <c r="E11" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="F11" t="s">
         <v>32</v>
@@ -732,16 +750,16 @@
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
-        <v>23</v>
+        <v>11</v>
       </c>
       <c r="B12" t="s">
+        <v>29</v>
+      </c>
+      <c r="C12" t="s">
         <v>30</v>
       </c>
-      <c r="C12" t="s">
-        <v>31</v>
-      </c>
       <c r="E12" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="F12" t="s">
         <v>32</v>
@@ -749,18 +767,35 @@
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
+        <v>23</v>
+      </c>
+      <c r="B13" t="s">
+        <v>30</v>
+      </c>
+      <c r="C13" t="s">
+        <v>31</v>
+      </c>
+      <c r="E13" t="s">
+        <v>21</v>
+      </c>
+      <c r="F13" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="14" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A14" t="s">
         <v>12</v>
       </c>
-      <c r="B13" t="s">
+      <c r="B14" t="s">
         <v>31</v>
       </c>
-      <c r="C13" t="s">
+      <c r="C14" t="s">
         <v>33</v>
       </c>
-      <c r="E13" t="s">
+      <c r="E14" t="s">
         <v>20</v>
       </c>
-      <c r="F13" t="s">
+      <c r="F14" t="s">
         <v>32</v>
       </c>
     </row>
@@ -774,7 +809,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A1014770-38FB-4B19-AD2D-C94E0AFBC5C4}">
   <dimension ref="A1:E2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="C6" sqref="C6"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
Update status task in sprint
</commit_message>
<xml_diff>
--- a/sprint_project.xlsx
+++ b/sprint_project.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Fadhlan\Pembelajaran Mesin\Tugas_Praktikum_ML_A_297-233\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\DATA 1\ARSIP TUGAS\ARSIP UMM\TUGAS KULIAH TEKNIK INFORMATIKA UMM\SEMESTER 7\PEMBELAJARAN MESIN 7A\MODUL PRAKTIKUM\TUGAS PRAK ML KELOMPOK\Tugas_Praktikum_ML_A_297-233\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BDA035D8-B585-426F-97E0-466EB705D078}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A66109CF-DC39-4361-A33D-B52D25918AAA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{5C1D3006-E29B-4E8A-AA24-3CECFF9100A6}"/>
   </bookViews>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="86" uniqueCount="44">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="87" uniqueCount="44">
   <si>
     <t>TASK</t>
   </si>
@@ -530,7 +530,7 @@
   <dimension ref="A1:F14"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F9" sqref="F9"/>
+      <selection activeCell="F6" sqref="F6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -633,11 +633,14 @@
       <c r="C5" s="3" t="s">
         <v>27</v>
       </c>
+      <c r="D5" t="s">
+        <v>41</v>
+      </c>
       <c r="E5" t="s">
         <v>21</v>
       </c>
       <c r="F5" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.3">

</xml_diff>

<commit_message>
update task and add new ipynb
</commit_message>
<xml_diff>
--- a/sprint_project.xlsx
+++ b/sprint_project.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24527"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24701"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\DATA 1\ARSIP TUGAS\ARSIP UMM\TUGAS KULIAH TEKNIK INFORMATIKA UMM\SEMESTER 7\PEMBELAJARAN MESIN 7A\MODUL PRAKTIKUM\TUGAS PRAK ML KELOMPOK\Tugas_Praktikum_ML_A_297-233\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Fadhlan\Pembelajaran Mesin\Tugas_Praktikum_ML_A_297-233\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F62F0D41-11C7-41AC-B164-5C9D10563A3C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7FA193E7-70A5-459A-8540-E0A03A2E6772}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{5C1D3006-E29B-4E8A-AA24-3CECFF9100A6}"/>
+    <workbookView xWindow="1272" yWindow="1392" windowWidth="17280" windowHeight="8964" xr2:uid="{5C1D3006-E29B-4E8A-AA24-3CECFF9100A6}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="93" uniqueCount="46">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="94" uniqueCount="47">
   <si>
     <t>TASK</t>
   </si>
@@ -164,6 +164,9 @@
   </si>
   <si>
     <t>ADD MORE IMAGE PROCESSING</t>
+  </si>
+  <si>
+    <t>7 Desember 2021</t>
   </si>
 </sst>
 </file>
@@ -171,7 +174,7 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="1">
-    <numFmt numFmtId="166" formatCode="[$-421]dd\ mmmm\ yyyy;@"/>
+    <numFmt numFmtId="164" formatCode="[$-421]dd\ mmmm\ yyyy;@"/>
   </numFmts>
   <fonts count="2" x14ac:knownFonts="1">
     <font>
@@ -222,7 +225,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
   </cellXfs>
@@ -542,7 +545,7 @@
   <dimension ref="A1:F15"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F14" sqref="F14"/>
+      <selection activeCell="D12" sqref="D12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -725,11 +728,14 @@
       <c r="C9" s="5">
         <v>44537</v>
       </c>
+      <c r="D9" t="s">
+        <v>46</v>
+      </c>
       <c r="E9" t="s">
         <v>20</v>
       </c>
       <c r="F9" t="s">
-        <v>43</v>
+        <v>34</v>
       </c>
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.3">

</xml_diff>